<commit_message>
Update to version 5.0.0
Major Version Update
</commit_message>
<xml_diff>
--- a/Maps/HOTAS Switch and Button - Quick Reference - BASIC.xlsx
+++ b/Maps/HOTAS Switch and Button - Quick Reference - BASIC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Den\OneDrive\Personal\Thrustmaster\TARGET\Clicker\Development\ED_TargetScript-430\Maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Den\OneDrive\Personal\Thrustmaster\TARGET\Clicker\Development\ED_TargetScript-500\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -368,7 +368,7 @@
     <t>TargetNextHostileShip</t>
   </si>
   <si>
-    <t>HOTAS - Quick reference - v4.3.0 - BASIC</t>
+    <t>HOTAS - Quick reference - v5.0.0 - BASIC</t>
   </si>
 </sst>
 </file>

</xml_diff>